<commit_message>
added regerssion for cart module
</commit_message>
<xml_diff>
--- a/manual_tests/Locators.xlsx
+++ b/manual_tests/Locators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ebfd5dc42167825/Desktop/Testing/Mamta_Mobiles/manual_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{5C7D3BD4-F4B4-49AF-B86C-38D278758476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65944ABC-A6CF-49C1-9565-F612768763ED}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{5C7D3BD4-F4B4-49AF-B86C-38D278758476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABBE90F2-9B95-477B-B67B-71348F1CE94C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3DCFDCF1-7723-4809-B984-9D29D92B5F9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
   <si>
     <t>Element Description</t>
   </si>
@@ -438,13 +438,220 @@
       </rPr>
       <t>class</t>
     </r>
+  </si>
+  <si>
+    <t>1. Product Details (for TC_CART_001)</t>
+  </si>
+  <si>
+    <r>
+      <t>Product Name:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g., The element containing "Samsung Galaxy S25 Ultra")</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Product Price:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g., The element containing "₹141,999")</t>
+    </r>
+  </si>
+  <si>
+    <t>2. Quantity Controls (for TC_CART_002)</t>
+  </si>
+  <si>
+    <r>
+      <t>Plus (+) Button:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (The button to increase quantity)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Quantity Display:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (The number showing "1" or "2" between the buttons)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Subtotal Price:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (The final calculated price at the bottom, e.g., "₹283,998")</t>
+    </r>
+  </si>
+  <si>
+    <t>3. Remove Item (for TC_CART_003)</t>
+  </si>
+  <si>
+    <r>
+      <t>Delete/Trash Button:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (The icon/button to remove the item)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Empty Cart Message:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (The text that appears after deletion, e.g., "Your cart is empty")</t>
+    </r>
+  </si>
+  <si>
+    <t>4. User Menu (for TC_CART_004 - Persistence)</t>
+  </si>
+  <si>
+    <r>
+      <t>Profile Icon/Menu:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (To access the Logout option)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Logout Button:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Inside the profile menu)</t>
+    </r>
+  </si>
+  <si>
+    <t>5. Navigation (for TC_CART_005)</t>
+  </si>
+  <si>
+    <r>
+      <t>Proceed to Checkout Button:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (We already have this: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>page.getByRole('button', { name: 'Proceed to Checkout' })</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>page.locator('h3:has-text("Samsung Galaxy S25 Ultra")')</t>
+  </si>
+  <si>
+    <t>page.locator('p:has-text("₹141,999")')</t>
+  </si>
+  <si>
+    <t>page.locator('span').filter({ hasText: '1' }).first()</t>
+  </si>
+  <si>
+    <t>page.getByText('₹167,558.82', { exact: true })</t>
+  </si>
+  <si>
+    <t>page.locator(".lucide.lucide-minus.w-3.h-3")</t>
+  </si>
+  <si>
+    <t>page.locator(".lucide.lucide-plus.w-3.h-3")</t>
+  </si>
+  <si>
+    <t>page.locator(".lucide.lucide-trash2.lucide-trash-2.w-4.h-4")</t>
+  </si>
+  <si>
+    <t>page.getByRole('button', { name: 'Logout' })</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,6 +687,19 @@
       <name val="Aptos Display"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -523,7 +743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
@@ -535,6 +755,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,6 +775,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -869,20 +1098,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EB169EB-7FCB-40FD-876C-AC66A4304570}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="34.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="34.21875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="92.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="107.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -893,7 +1122,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -904,7 +1133,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -915,7 +1144,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -926,7 +1155,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -937,7 +1166,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -948,7 +1177,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -959,7 +1188,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -970,7 +1199,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="43.2">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -981,7 +1210,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -992,7 +1221,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1003,7 +1232,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="43.2">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1014,7 +1243,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -1025,7 +1254,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -1036,7 +1265,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -1047,7 +1276,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -1058,14 +1287,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -1076,7 +1305,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="28.8">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1087,7 +1316,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
@@ -1096,7 +1325,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
@@ -1105,7 +1334,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" s="4" t="s">
         <v>41</v>
       </c>
@@ -1114,7 +1343,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" s="4" t="s">
         <v>42</v>
       </c>
@@ -1123,7 +1352,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
@@ -1131,6 +1360,129 @@
       <c r="C24" s="4" t="s">
         <v>44</v>
       </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>